<commit_message>
ML and Data Science
</commit_message>
<xml_diff>
--- a/1_Probability_and_Statistics/Statistics/_12_Std_Normal_Distribution/3.4.Standard-normal-distribution-exercise.xlsx
+++ b/1_Probability_and_Statistics/Statistics/_12_Std_Normal_Distribution/3.4.Standard-normal-distribution-exercise.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data_science_bootcamp\Resources\Part_3_Statistics\S17_L99\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siddarth\Desktop\Machine_Learning_and_Data_Science\1_Probability_and_Statistics\Statistics\_12_Std_Normal_Distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B4534A-F718-4E28-971C-8ECC3B446903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB52B937-8055-4A98-AEA6-C7BB99F394BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1502,7 +1502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -2249,7 +2249,7 @@
       <c r="N27" s="7"/>
       <c r="P27" s="7"/>
       <c r="Q27" s="30">
-        <f>I27/$E$11</f>
+        <f t="shared" ref="Q27:Q58" si="1">I27/$E$11</f>
         <v>-0.9092760935373293</v>
       </c>
       <c r="R27" s="7"/>
@@ -2277,7 +2277,7 @@
       <c r="N28" s="7"/>
       <c r="P28" s="7"/>
       <c r="Q28" s="30">
-        <f>I28/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.77743570819313035</v>
       </c>
       <c r="R28" s="7"/>
@@ -2311,7 +2311,7 @@
       <c r="N29" s="7"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="30">
-        <f>I29/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.65911741365346466</v>
       </c>
       <c r="R29" s="7"/>
@@ -2353,7 +2353,7 @@
       <c r="N30" s="7"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="30">
-        <f>I30/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.61404377763835183</v>
       </c>
       <c r="R30" s="7"/>
@@ -2395,7 +2395,7 @@
       <c r="N31" s="7"/>
       <c r="P31" s="7"/>
       <c r="Q31" s="30">
-        <f>I31/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.5036133694013325</v>
       </c>
       <c r="R31" s="7"/>
@@ -2437,7 +2437,7 @@
       <c r="N32" s="7"/>
       <c r="P32" s="7"/>
       <c r="Q32" s="30">
-        <f>I32/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.50248652850095266</v>
       </c>
       <c r="R32" s="7"/>
@@ -2479,7 +2479,7 @@
       <c r="N33" s="7"/>
       <c r="P33" s="7"/>
       <c r="Q33" s="30">
-        <f>I33/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.47206182419075293</v>
       </c>
       <c r="R33" s="7"/>
@@ -2521,7 +2521,7 @@
       <c r="N34" s="7"/>
       <c r="P34" s="7"/>
       <c r="Q34" s="30">
-        <f>I34/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.43262239267753305</v>
       </c>
       <c r="R34" s="7"/>
@@ -2563,7 +2563,7 @@
       <c r="N35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="30">
-        <f>I35/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.39205612026393338</v>
       </c>
       <c r="R35" s="7"/>
@@ -2605,7 +2605,7 @@
       <c r="N36" s="7"/>
       <c r="P36" s="7"/>
       <c r="Q36" s="30">
-        <f>I36/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.36501193865486692</v>
       </c>
       <c r="R36" s="7"/>
@@ -2647,7 +2647,7 @@
       <c r="N37" s="7"/>
       <c r="P37" s="7"/>
       <c r="Q37" s="30">
-        <f>I37/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.28049887112653427</v>
       </c>
       <c r="R37" s="7"/>
@@ -2689,7 +2689,7 @@
       <c r="N38" s="7"/>
       <c r="P38" s="7"/>
       <c r="Q38" s="30">
-        <f>I38/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.2016200081000884</v>
       </c>
       <c r="R38" s="7"/>
@@ -2727,7 +2727,7 @@
       <c r="N39" s="7"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="30">
-        <f>I39/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.19373212179744503</v>
       </c>
       <c r="R39" s="7"/>
@@ -2755,7 +2755,7 @@
       <c r="N40" s="7"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="30">
-        <f>I40/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.18922475819593498</v>
       </c>
       <c r="R40" s="7"/>
@@ -2783,7 +2783,7 @@
       <c r="N41" s="7"/>
       <c r="P41" s="7"/>
       <c r="Q41" s="30">
-        <f>I41/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.17457582649102193</v>
       </c>
       <c r="R41" s="7"/>
@@ -2811,7 +2811,7 @@
       <c r="N42" s="7"/>
       <c r="P42" s="7"/>
       <c r="Q42" s="30">
-        <f>I42/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.14978532668271205</v>
       </c>
       <c r="R42" s="7"/>
@@ -2839,7 +2839,7 @@
       <c r="N43" s="7"/>
       <c r="P43" s="7"/>
       <c r="Q43" s="30">
-        <f>I43/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-0.10809221336873563</v>
       </c>
       <c r="R43" s="7"/>
@@ -2867,7 +2867,7 @@
       <c r="N44" s="7"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="30">
-        <f>I44/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-8.2174872660045931E-2</v>
       </c>
       <c r="R44" s="7"/>
@@ -2895,7 +2895,7 @@
       <c r="N45" s="7"/>
       <c r="P45" s="7"/>
       <c r="Q45" s="30">
-        <f>I45/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-7.654066815815605E-2</v>
       </c>
       <c r="R45" s="7"/>
@@ -2923,7 +2923,7 @@
       <c r="N46" s="7"/>
       <c r="P46" s="7"/>
       <c r="Q46" s="30">
-        <f>I46/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-6.4145418254002648E-2</v>
       </c>
       <c r="R46" s="7"/>
@@ -2951,7 +2951,7 @@
       <c r="N47" s="7"/>
       <c r="P47" s="7"/>
       <c r="Q47" s="30">
-        <f>I47/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-4.3862282047202807E-2</v>
       </c>
       <c r="R47" s="7"/>
@@ -2981,7 +2981,7 @@
       <c r="N48" s="7"/>
       <c r="P48" s="7"/>
       <c r="Q48" s="30">
-        <f>I48/$E$11</f>
+        <f t="shared" si="1"/>
         <v>-3.2593873043423073E-2</v>
       </c>
       <c r="R48" s="7"/>
@@ -3011,7 +3011,7 @@
       <c r="N49" s="7"/>
       <c r="P49" s="7"/>
       <c r="Q49" s="30">
-        <f>I49/$E$11</f>
+        <f t="shared" si="1"/>
         <v>7.9723993701766097E-3</v>
       </c>
       <c r="R49" s="7"/>
@@ -3041,7 +3041,7 @@
       <c r="N50" s="7"/>
       <c r="P50" s="7"/>
       <c r="Q50" s="30">
-        <f>I50/$E$11</f>
+        <f t="shared" si="1"/>
         <v>5.6426558086419644E-2</v>
       </c>
       <c r="R50" s="7"/>
@@ -3071,7 +3071,7 @@
       <c r="N51" s="7"/>
       <c r="P51" s="7"/>
       <c r="Q51" s="30">
-        <f>I51/$E$11</f>
+        <f t="shared" si="1"/>
         <v>6.9948648890952869E-2</v>
       </c>
       <c r="R51" s="7"/>
@@ -3101,7 +3101,7 @@
       <c r="N52" s="7"/>
       <c r="P52" s="7"/>
       <c r="Q52" s="30">
-        <f>I52/$E$11</f>
+        <f t="shared" si="1"/>
         <v>7.1075489791329619E-2</v>
       </c>
       <c r="R52" s="7"/>
@@ -3131,7 +3131,7 @@
       <c r="N53" s="7"/>
       <c r="P53" s="7"/>
       <c r="Q53" s="30">
-        <f>I53/$E$11</f>
+        <f t="shared" si="1"/>
         <v>7.445601249246292E-2</v>
       </c>
       <c r="R53" s="7"/>
@@ -3161,7 +3161,7 @@
       <c r="N54" s="7"/>
       <c r="P54" s="7"/>
       <c r="Q54" s="30">
-        <f>I54/$E$11</f>
+        <f t="shared" si="1"/>
         <v>9.4739148699262768E-2</v>
       </c>
       <c r="R54" s="7"/>
@@ -3191,7 +3191,7 @@
       <c r="N55" s="7"/>
       <c r="P55" s="7"/>
       <c r="Q55" s="30">
-        <f>I55/$E$11</f>
+        <f t="shared" si="1"/>
         <v>0.12291017120870903</v>
       </c>
       <c r="R55" s="7"/>
@@ -3221,7 +3221,7 @@
       <c r="N56" s="7"/>
       <c r="P56" s="7"/>
       <c r="Q56" s="30">
-        <f>I56/$E$11</f>
+        <f t="shared" si="1"/>
         <v>0.15784223912041884</v>
       </c>
       <c r="R56" s="7"/>
@@ -3251,7 +3251,7 @@
       <c r="N57" s="7"/>
       <c r="P57" s="7"/>
       <c r="Q57" s="30">
-        <f>I57/$E$11</f>
+        <f t="shared" si="1"/>
         <v>0.16234960272192889</v>
       </c>
       <c r="R57" s="7"/>
@@ -3281,7 +3281,7 @@
       <c r="N58" s="7"/>
       <c r="P58" s="7"/>
       <c r="Q58" s="30">
-        <f>I58/$E$11</f>
+        <f t="shared" si="1"/>
         <v>0.20742323873704016</v>
       </c>
       <c r="R58" s="7"/>
@@ -3311,7 +3311,7 @@
       <c r="N59" s="7"/>
       <c r="P59" s="7"/>
       <c r="Q59" s="30">
-        <f>I59/$E$11</f>
+        <f t="shared" ref="Q59:Q90" si="2">I59/$E$11</f>
         <v>0.23672110214686318</v>
       </c>
       <c r="R59" s="7"/>
@@ -3341,7 +3341,7 @@
       <c r="N60" s="7"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="30">
-        <f>I60/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.28404841996272945</v>
       </c>
       <c r="R60" s="7"/>
@@ -3371,7 +3371,7 @@
       <c r="N61" s="7"/>
       <c r="P61" s="7"/>
       <c r="Q61" s="30">
-        <f>I61/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.3550393966865289</v>
       </c>
       <c r="R61" s="7"/>
@@ -3401,7 +3401,7 @@
       <c r="N62" s="7"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="30">
-        <f>I62/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.43842562331448326</v>
       </c>
       <c r="R62" s="7"/>
@@ -3431,7 +3431,7 @@
       <c r="N63" s="7"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="30">
-        <f>I63/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.51617764544054934</v>
       </c>
       <c r="R63" s="7"/>
@@ -3461,7 +3461,7 @@
       <c r="N64" s="7"/>
       <c r="P64" s="7"/>
       <c r="Q64" s="30">
-        <f>I64/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.52293869084281597</v>
       </c>
       <c r="R64" s="7"/>
@@ -3491,7 +3491,7 @@
       <c r="N65" s="7"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="30">
-        <f>I65/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.57590021316057061</v>
       </c>
       <c r="R65" s="7"/>
@@ -3521,7 +3521,7 @@
       <c r="N66" s="7"/>
       <c r="P66" s="7"/>
       <c r="Q66" s="30">
-        <f>I66/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.67280853059305967</v>
       </c>
       <c r="R66" s="7"/>
@@ -3551,7 +3551,7 @@
       <c r="N67" s="7"/>
       <c r="P67" s="7"/>
       <c r="Q67" s="30">
-        <f>I67/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.68069641689570304</v>
       </c>
       <c r="R67" s="7"/>
@@ -3581,7 +3581,7 @@
       <c r="N68" s="7"/>
       <c r="P68" s="7"/>
       <c r="Q68" s="30">
-        <f>I68/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.70661375760439282</v>
       </c>
       <c r="R68" s="7"/>
@@ -3611,7 +3611,7 @@
       <c r="N69" s="7"/>
       <c r="P69" s="7"/>
       <c r="Q69" s="30">
-        <f>I69/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.73816530281496928</v>
       </c>
       <c r="R69" s="7"/>
@@ -3641,7 +3641,7 @@
       <c r="N70" s="7"/>
       <c r="P70" s="7"/>
       <c r="Q70" s="30">
-        <f>I70/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.75619475722101415</v>
       </c>
       <c r="R70" s="7"/>
@@ -3671,7 +3671,7 @@
       <c r="N71" s="7"/>
       <c r="P71" s="7"/>
       <c r="Q71" s="30">
-        <f>I71/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.76633632532441398</v>
       </c>
       <c r="R71" s="7"/>
@@ -3701,7 +3701,7 @@
       <c r="N72" s="7"/>
       <c r="P72" s="7"/>
       <c r="Q72" s="30">
-        <f>I72/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.7697168480255473</v>
       </c>
       <c r="R72" s="7"/>
@@ -3731,7 +3731,7 @@
       <c r="N73" s="7"/>
       <c r="P73" s="7"/>
       <c r="Q73" s="30">
-        <f>I73/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.91733300597503453</v>
       </c>
       <c r="R73" s="7"/>
@@ -3761,7 +3761,7 @@
       <c r="N74" s="7"/>
       <c r="P74" s="7"/>
       <c r="Q74" s="30">
-        <f>I74/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.92634773317805774</v>
       </c>
       <c r="R74" s="7"/>
@@ -3791,7 +3791,7 @@
       <c r="N75" s="7"/>
       <c r="P75" s="7"/>
       <c r="Q75" s="30">
-        <f>I75/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.95451875568750089</v>
       </c>
       <c r="R75" s="7"/>
@@ -3821,7 +3821,7 @@
       <c r="N76" s="7"/>
       <c r="P76" s="7"/>
       <c r="Q76" s="30">
-        <f>I76/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.96015296018939078</v>
       </c>
       <c r="R76" s="7"/>
@@ -3851,7 +3851,7 @@
       <c r="N77" s="7"/>
       <c r="P77" s="7"/>
       <c r="Q77" s="30">
-        <f>I77/$E$11</f>
+        <f t="shared" si="2"/>
         <v>0.97029452829279073</v>
       </c>
       <c r="R77" s="7"/>
@@ -3881,7 +3881,7 @@
       <c r="N78" s="7"/>
       <c r="P78" s="7"/>
       <c r="Q78" s="30">
-        <f>I78/$E$11</f>
+        <f t="shared" si="2"/>
         <v>1.011987641606767</v>
       </c>
       <c r="R78" s="7"/>
@@ -3911,7 +3911,7 @@
       <c r="N79" s="7"/>
       <c r="P79" s="7"/>
       <c r="Q79" s="30">
-        <f>I79/$E$11</f>
+        <f t="shared" si="2"/>
         <v>1.0255097324113003</v>
       </c>
       <c r="R79" s="7"/>
@@ -3941,7 +3941,7 @@
       <c r="N80" s="7"/>
       <c r="P80" s="7"/>
       <c r="Q80" s="30">
-        <f>I80/$E$11</f>
+        <f t="shared" si="2"/>
         <v>1.0503002322196118</v>
       </c>
       <c r="R80" s="7"/>
@@ -3971,7 +3971,7 @@
       <c r="N81" s="7"/>
       <c r="P81" s="7"/>
       <c r="Q81" s="30">
-        <f>I81/$E$11</f>
+        <f t="shared" si="2"/>
         <v>1.0559344367215</v>
       </c>
       <c r="R81" s="7"/>
@@ -4001,7 +4001,7 @@
       <c r="N82" s="7"/>
       <c r="P82" s="7"/>
       <c r="Q82" s="30">
-        <f>I82/$E$11</f>
+        <f t="shared" si="2"/>
         <v>1.1167838453418997</v>
       </c>
       <c r="R82" s="7"/>
@@ -4031,7 +4031,7 @@
       <c r="N83" s="7"/>
       <c r="P83" s="7"/>
       <c r="Q83" s="30">
-        <f>I83/$E$11</f>
+        <f t="shared" si="2"/>
         <v>1.1573501177554992</v>
       </c>
       <c r="R83" s="7"/>
@@ -4052,7 +4052,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
       <c r="I84" s="28">
-        <f t="shared" ref="I84:I90" si="1">B84-$E$10</f>
+        <f t="shared" ref="I84:I90" si="3">B84-$E$10</f>
         <v>98.422916666666879</v>
       </c>
       <c r="K84" s="7"/>
@@ -4061,7 +4061,7 @@
       <c r="N84" s="7"/>
       <c r="P84" s="7"/>
       <c r="Q84" s="30">
-        <f>I84/$E$11</f>
+        <f t="shared" si="2"/>
         <v>1.3308836164136761</v>
       </c>
       <c r="R84" s="7"/>
@@ -4082,7 +4082,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
       <c r="I85" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>99.00625000000025</v>
       </c>
       <c r="K85" s="7"/>
@@ -4091,7 +4091,7 @@
       <c r="N85" s="7"/>
       <c r="P85" s="7"/>
       <c r="Q85" s="30">
-        <f>I85/$E$11</f>
+        <f t="shared" si="2"/>
         <v>1.3387715027163212</v>
       </c>
       <c r="R85" s="7"/>
@@ -4112,7 +4112,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
       <c r="I86" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>99.839583333333508</v>
       </c>
       <c r="K86" s="7"/>
@@ -4121,7 +4121,7 @@
       <c r="N86" s="7"/>
       <c r="P86" s="7"/>
       <c r="Q86" s="30">
-        <f>I86/$E$11</f>
+        <f t="shared" si="2"/>
         <v>1.3500399117200979</v>
       </c>
       <c r="R86" s="7"/>
@@ -4142,7 +4142,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
       <c r="I87" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>106.58958333333351</v>
       </c>
       <c r="K87" s="7"/>
@@ -4151,7 +4151,7 @@
       <c r="N87" s="7"/>
       <c r="P87" s="7"/>
       <c r="Q87" s="30">
-        <f>I87/$E$11</f>
+        <f t="shared" si="2"/>
         <v>1.441314024650697</v>
       </c>
       <c r="R87" s="7"/>
@@ -4172,7 +4172,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
       <c r="I88" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>131.67291666666688</v>
       </c>
       <c r="K88" s="7"/>
@@ -4181,7 +4181,7 @@
       <c r="N88" s="7"/>
       <c r="P88" s="7"/>
       <c r="Q88" s="30">
-        <f>I88/$E$11</f>
+        <f t="shared" si="2"/>
         <v>1.780493135664406</v>
       </c>
       <c r="R88" s="7"/>
@@ -4202,7 +4202,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
       <c r="I89" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>135.75625000000025</v>
       </c>
       <c r="K89" s="7"/>
@@ -4211,7 +4211,7 @@
       <c r="N89" s="7"/>
       <c r="P89" s="7"/>
       <c r="Q89" s="30">
-        <f>I89/$E$11</f>
+        <f t="shared" si="2"/>
         <v>1.8357083397829173</v>
       </c>
       <c r="R89" s="7"/>
@@ -4232,7 +4232,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
       <c r="I90" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>154.42291666666688</v>
       </c>
       <c r="K90" s="7"/>
@@ -4241,7 +4241,7 @@
       <c r="N90" s="7"/>
       <c r="P90" s="7"/>
       <c r="Q90" s="32">
-        <f>I90/$E$11</f>
+        <f t="shared" si="2"/>
         <v>2.0881207014675369</v>
       </c>
       <c r="R90" s="7"/>

</xml_diff>